<commit_message>
updated 2024 PITcleanr output. Assigned user_keep_obs myself
</commit_message>
<xml_diff>
--- a/outgoing/PITcleanr/PRO_Steelhead_2024.xlsx
+++ b/outgoing/PITcleanr/PRO_Steelhead_2024.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://stateofwa-my.sharepoint.com/personal/kevin_see_dfw_wa_gov/Documents/Documents/Git/MyProjects/DabomYakimaSthd/outgoing/PITcleanr/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="11_156EDDCC8F79A89360642C52EA7BD2721AC83D19" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BE5E9F56-BDA0-45AF-ADCF-59A2C1D787BC}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="11_B466DDCC8F79A89360642C52EA7BD272EAC75A6D" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{72509B56-A81C-4DEF-98C0-3201BF1D1800}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1143,8 +1143,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P336"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
-      <selection activeCell="A91" sqref="A91"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>